<commit_message>
uploading respiration and emergence data
</commit_message>
<xml_diff>
--- a/data/Respiration_tracker.xlsx
+++ b/data/Respiration_tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chloegilligan/Desktop/Repositories/Nucella_2025/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{70D34428-0B15-6240-867B-5DC5ED37A84B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{791B6884-9C82-3D49-A217-3205DD49B9C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{374850A1-0577-BF46-9074-5B5F9242F0BC}"/>
+    <workbookView xWindow="260" yWindow="2700" windowWidth="27640" windowHeight="16940" xr2:uid="{374850A1-0577-BF46-9074-5B5F9242F0BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="105">
   <si>
     <t>Full Sample ID</t>
   </si>
@@ -313,16 +313,65 @@
   <si>
     <t>Respiration trial 3
  Heated</t>
+  </si>
+  <si>
+    <t>AFDW ID and date</t>
+  </si>
+  <si>
+    <t>BRP2_A1_20250716</t>
+  </si>
+  <si>
+    <t>BRP3_A2_20250716</t>
+  </si>
+  <si>
+    <t>RIG2_A3_20250716</t>
+  </si>
+  <si>
+    <t>RIR4_A4_20250716</t>
+  </si>
+  <si>
+    <t>RIP4_A5_20250716</t>
+  </si>
+  <si>
+    <t>RIP3_A6_20250716</t>
+  </si>
+  <si>
+    <t>RIR2_B1_20250716</t>
+  </si>
+  <si>
+    <t>RIP5_B6_20250716</t>
+  </si>
+  <si>
+    <t>BRP4_C1_20250716</t>
+  </si>
+  <si>
+    <t>RIP2_C3_20250716</t>
+  </si>
+  <si>
+    <t>BRR4_D3_20250716</t>
+  </si>
+  <si>
+    <t>Castle rock</t>
+  </si>
+  <si>
+    <t>Dead</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -360,7 +409,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -695,10 +744,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C0A0720-605D-1742-87B3-D617BE040EF1}">
-  <dimension ref="A1:L73"/>
+  <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F73"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="163" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J74" sqref="J74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -710,9 +760,10 @@
     <col min="10" max="10" width="15.33203125" customWidth="1"/>
     <col min="11" max="11" width="17.5" customWidth="1"/>
     <col min="12" max="12" width="16.1640625" customWidth="1"/>
+    <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -749,24 +800,51 @@
       <c r="L1" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>20250716</v>
+      </c>
+      <c r="F2">
+        <v>20250718</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>20250716</v>
+      </c>
+      <c r="F3">
+        <v>20250716</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -782,8 +860,11 @@
       <c r="E4">
         <v>20250714</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <v>20250718</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -803,15 +884,24 @@
         <v>20250714</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>20250718</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -827,16 +917,31 @@
       <c r="E7">
         <v>20250714</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <v>20250716</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>20250716</v>
+      </c>
+      <c r="F8">
+        <v>20250721</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -856,7 +961,7 @@
         <v>20250711</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -872,8 +977,11 @@
       <c r="E10">
         <v>20250709</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F10">
+        <v>20250721</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -893,7 +1001,7 @@
         <v>20250709</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -909,8 +1017,11 @@
       <c r="E12">
         <v>20250711</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F12">
+        <v>20250716</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -930,7 +1041,7 @@
         <v>20250709</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -946,8 +1057,11 @@
       <c r="E14">
         <v>20250714</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F14">
+        <v>20250716</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -967,15 +1081,27 @@
         <v>20250709</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>25</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>20250716</v>
+      </c>
+      <c r="F16">
+        <v>20250716</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -991,8 +1117,11 @@
       <c r="E17">
         <v>20250709</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F17">
+        <v>20250716</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1008,16 +1137,31 @@
       <c r="E18">
         <v>20250714</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>28</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>20250718</v>
+      </c>
+      <c r="F19">
+        <v>20250718</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -1033,8 +1177,11 @@
       <c r="E20">
         <v>20250714</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F20">
+        <v>20250716</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1042,7 +1189,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -1050,7 +1197,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -1066,16 +1213,31 @@
       <c r="E23">
         <v>20250714</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F23">
+        <v>20250716</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>33</v>
       </c>
       <c r="B24" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24">
+        <v>6</v>
+      </c>
+      <c r="E24">
+        <v>20250718</v>
+      </c>
+      <c r="F24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -1091,8 +1253,11 @@
       <c r="E25">
         <v>20250714</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -1112,7 +1277,7 @@
         <v>20250711</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -1132,23 +1297,44 @@
         <v>20250711</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>38</v>
       </c>
       <c r="B28" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>20250718</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>39</v>
       </c>
       <c r="B29" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>20250718</v>
+      </c>
+      <c r="F29">
+        <v>20250718</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -1167,8 +1353,14 @@
       <c r="F30">
         <v>20250714</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30">
+        <v>20250718</v>
+      </c>
+      <c r="H30">
+        <v>20250718</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -1181,14 +1373,26 @@
       <c r="D31">
         <v>2</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E31">
         <v>20250630</v>
       </c>
       <c r="F31">
         <v>20250704</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31">
+        <v>20250716</v>
+      </c>
+      <c r="H31" s="3">
+        <v>20250716</v>
+      </c>
+      <c r="I31">
+        <v>20250718</v>
+      </c>
+      <c r="M31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -1201,14 +1405,26 @@
       <c r="D32">
         <v>2</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32">
         <v>20250704</v>
       </c>
       <c r="F32">
         <v>20250704</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32">
+        <v>20250716</v>
+      </c>
+      <c r="H32" s="3">
+        <v>20250716</v>
+      </c>
+      <c r="I32">
+        <v>20250718</v>
+      </c>
+      <c r="M32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>43</v>
       </c>
@@ -1221,14 +1437,26 @@
       <c r="D33">
         <v>2</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33">
         <v>20250630</v>
       </c>
       <c r="F33">
         <v>20250702</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33" s="3">
+        <v>20250716</v>
+      </c>
+      <c r="H33" s="3">
+        <v>20250716</v>
+      </c>
+      <c r="I33">
+        <v>20250718</v>
+      </c>
+      <c r="M33" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>44</v>
       </c>
@@ -1238,8 +1466,11 @@
       <c r="E34">
         <v>20250709</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F34">
+        <v>20250718</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>45</v>
       </c>
@@ -1256,7 +1487,7 @@
         <v>20250709</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>46</v>
       </c>
@@ -1276,7 +1507,7 @@
         <v>20250709</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>47</v>
       </c>
@@ -1289,14 +1520,26 @@
       <c r="D37">
         <v>3</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E37">
         <v>20250704</v>
       </c>
       <c r="F37">
         <v>20250707</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G37">
+        <v>20250716</v>
+      </c>
+      <c r="H37">
+        <v>20250716</v>
+      </c>
+      <c r="I37" s="3">
+        <v>20250718</v>
+      </c>
+      <c r="M37" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>48</v>
       </c>
@@ -1312,8 +1555,17 @@
       <c r="E38">
         <v>20250707</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F38">
+        <v>20250716</v>
+      </c>
+      <c r="G38">
+        <v>20250718</v>
+      </c>
+      <c r="H38">
+        <v>20250718</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>49</v>
       </c>
@@ -1326,14 +1578,23 @@
       <c r="D39">
         <v>4</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E39">
         <v>20250702</v>
       </c>
-      <c r="F39" s="3">
+      <c r="F39">
         <v>20250702</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G39">
+        <v>20250716</v>
+      </c>
+      <c r="H39">
+        <v>20250716</v>
+      </c>
+      <c r="M39" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>50</v>
       </c>
@@ -1349,8 +1610,14 @@
       <c r="E40">
         <v>20250707</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G40">
+        <v>20250718</v>
+      </c>
+      <c r="H40">
+        <v>20250718</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>51</v>
       </c>
@@ -1363,14 +1630,26 @@
       <c r="D41">
         <v>4</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E41">
         <v>20250702</v>
       </c>
       <c r="F41">
         <v>20250702</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G41">
+        <v>20250716</v>
+      </c>
+      <c r="H41" s="3">
+        <v>20250716</v>
+      </c>
+      <c r="I41">
+        <v>20250718</v>
+      </c>
+      <c r="M41" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>52</v>
       </c>
@@ -1387,7 +1666,7 @@
         <v>20250711</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>53</v>
       </c>
@@ -1404,15 +1683,27 @@
         <v>20250709</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>54</v>
       </c>
       <c r="B44" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C44" t="s">
+        <v>36</v>
+      </c>
+      <c r="D44">
+        <v>5</v>
+      </c>
+      <c r="E44">
+        <v>20250716</v>
+      </c>
+      <c r="F44">
+        <v>20250716</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>55</v>
       </c>
@@ -1425,14 +1716,26 @@
       <c r="D45">
         <v>5</v>
       </c>
-      <c r="E45" s="2">
+      <c r="E45">
         <v>20250704</v>
       </c>
       <c r="F45">
         <v>20250707</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G45">
+        <v>20250716</v>
+      </c>
+      <c r="H45" s="3">
+        <v>20250716</v>
+      </c>
+      <c r="I45">
+        <v>20250718</v>
+      </c>
+      <c r="M45" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>56</v>
       </c>
@@ -1440,23 +1743,47 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>57</v>
       </c>
       <c r="B47" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C47" t="s">
+        <v>36</v>
+      </c>
+      <c r="D47">
+        <v>6</v>
+      </c>
+      <c r="E47">
+        <v>20250716</v>
+      </c>
+      <c r="F47">
+        <v>20250718</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>58</v>
       </c>
       <c r="B48" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C48" t="s">
+        <v>36</v>
+      </c>
+      <c r="D48">
+        <v>6</v>
+      </c>
+      <c r="E48">
+        <v>20250718</v>
+      </c>
+      <c r="F48">
+        <v>20250721</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>59</v>
       </c>
@@ -1476,7 +1803,7 @@
         <v>20250714</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>60</v>
       </c>
@@ -1496,7 +1823,7 @@
         <v>20250711</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>62</v>
       </c>
@@ -1504,7 +1831,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>63</v>
       </c>
@@ -1520,8 +1847,11 @@
       <c r="E52">
         <v>20250714</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F52">
+        <v>20250716</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>64</v>
       </c>
@@ -1540,8 +1870,14 @@
       <c r="F53">
         <v>20250714</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G53">
+        <v>20250718</v>
+      </c>
+      <c r="H53">
+        <v>20250718</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>65</v>
       </c>
@@ -1560,8 +1896,14 @@
       <c r="F54">
         <v>20250709</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G54">
+        <v>20250716</v>
+      </c>
+      <c r="H54">
+        <v>20250716</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>66</v>
       </c>
@@ -1580,8 +1922,14 @@
       <c r="F55">
         <v>20250714</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G55">
+        <v>20250718</v>
+      </c>
+      <c r="H55">
+        <v>20250718</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>67</v>
       </c>
@@ -1597,8 +1945,11 @@
       <c r="E56">
         <v>20250714</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F56">
+        <v>20250721</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>68</v>
       </c>
@@ -1611,14 +1962,26 @@
       <c r="D57">
         <v>2</v>
       </c>
-      <c r="E57" s="2">
+      <c r="E57">
         <v>20250704</v>
       </c>
       <c r="F57">
         <v>20250704</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G57">
+        <v>20250716</v>
+      </c>
+      <c r="H57">
+        <v>20250716</v>
+      </c>
+      <c r="I57" s="3">
+        <v>20250718</v>
+      </c>
+      <c r="M57" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>69</v>
       </c>
@@ -1638,7 +2001,7 @@
         <v>20250709</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>70</v>
       </c>
@@ -1654,16 +2017,35 @@
       <c r="E59">
         <v>20250707</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F59">
+        <v>20250716</v>
+      </c>
+      <c r="G59">
+        <v>20250718</v>
+      </c>
+      <c r="H59" s="2"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>71</v>
       </c>
       <c r="B60" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C60" t="s">
+        <v>61</v>
+      </c>
+      <c r="D60">
+        <v>3</v>
+      </c>
+      <c r="E60">
+        <v>20250718</v>
+      </c>
+      <c r="F60">
+        <v>20250718</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>72</v>
       </c>
@@ -1676,11 +2058,26 @@
       <c r="D61">
         <v>3</v>
       </c>
-      <c r="E61" s="2">
+      <c r="E61">
         <v>20250704</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F61" t="s">
+        <v>104</v>
+      </c>
+      <c r="G61">
+        <v>20250716</v>
+      </c>
+      <c r="H61">
+        <v>20250716</v>
+      </c>
+      <c r="I61" s="3">
+        <v>20250718</v>
+      </c>
+      <c r="M61" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>73</v>
       </c>
@@ -1696,8 +2093,11 @@
       <c r="E62">
         <v>20250711</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F62">
+        <v>20250721</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>74</v>
       </c>
@@ -1710,14 +2110,26 @@
       <c r="D63">
         <v>4</v>
       </c>
-      <c r="E63" s="2">
+      <c r="E63">
         <v>20250704</v>
       </c>
       <c r="F63">
         <v>20250704</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G63" s="3">
+        <v>20250716</v>
+      </c>
+      <c r="H63" s="3">
+        <v>20250716</v>
+      </c>
+      <c r="I63">
+        <v>20250718</v>
+      </c>
+      <c r="M63" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>75</v>
       </c>
@@ -1737,7 +2149,7 @@
         <v>20250714</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>76</v>
       </c>
@@ -1750,35 +2162,86 @@
       <c r="D65">
         <v>4</v>
       </c>
-      <c r="E65" s="2">
+      <c r="E65">
         <v>20250704</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F65">
+        <v>20250718</v>
+      </c>
+      <c r="G65" s="3">
+        <v>20250716</v>
+      </c>
+      <c r="H65">
+        <v>20250716</v>
+      </c>
+      <c r="I65">
+        <v>20250718</v>
+      </c>
+      <c r="M65" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>77</v>
       </c>
       <c r="B66" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C66" t="s">
+        <v>61</v>
+      </c>
+      <c r="D66">
+        <v>4</v>
+      </c>
+      <c r="E66">
+        <v>20250716</v>
+      </c>
+      <c r="F66">
+        <v>20250721</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>78</v>
       </c>
       <c r="B67" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C67" t="s">
+        <v>61</v>
+      </c>
+      <c r="D67">
+        <v>4</v>
+      </c>
+      <c r="E67">
+        <v>20250716</v>
+      </c>
+      <c r="F67">
+        <v>20250716</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>79</v>
       </c>
       <c r="B68" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C68" t="s">
+        <v>61</v>
+      </c>
+      <c r="D68">
+        <v>4</v>
+      </c>
+      <c r="E68">
+        <v>20250716</v>
+      </c>
+      <c r="F68">
+        <v>20250721</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>80</v>
       </c>
@@ -1794,8 +2257,11 @@
       <c r="E69">
         <v>20250714</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F69">
+        <v>20250716</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>81</v>
       </c>
@@ -1815,7 +2281,7 @@
         <v>20250711</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>82</v>
       </c>
@@ -1835,7 +2301,7 @@
         <v>20250714</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>83</v>
       </c>
@@ -1852,7 +2318,7 @@
         <v>20250714</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>84</v>
       </c>
@@ -1870,6 +2336,9 @@
       </c>
       <c r="F73">
         <v>20250707</v>
+      </c>
+      <c r="G73">
+        <v>20250718</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating nucella respiration data
</commit_message>
<xml_diff>
--- a/data/Respiration_tracker.xlsx
+++ b/data/Respiration_tracker.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chloegilligan/Desktop/Repositories/Nucella_2025/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{791B6884-9C82-3D49-A217-3205DD49B9C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24AE50F1-8751-2448-BAE1-706A42D5D4D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="2700" windowWidth="27640" windowHeight="16940" xr2:uid="{374850A1-0577-BF46-9074-5B5F9242F0BC}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="20000" windowHeight="18900" activeTab="2" xr2:uid="{374850A1-0577-BF46-9074-5B5F9242F0BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="108">
   <si>
     <t>Full Sample ID</t>
   </si>
@@ -355,6 +357,15 @@
   </si>
   <si>
     <t>Dead</t>
+  </si>
+  <si>
+    <t>RUN 3</t>
+  </si>
+  <si>
+    <t>RUN3</t>
+  </si>
+  <si>
+    <t>RUN 4</t>
   </si>
 </sst>
 </file>
@@ -377,7 +388,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -387,6 +398,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -403,13 +438,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -746,9 +787,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C0A0720-605D-1742-87B3-D617BE040EF1}">
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="163" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J74" sqref="J74"/>
+    <sheetView zoomScale="89" zoomScaleNormal="163" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:M73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -900,6 +941,9 @@
       <c r="E6">
         <v>20250718</v>
       </c>
+      <c r="F6">
+        <v>20250725</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1188,6 +1232,18 @@
       <c r="B21" t="s">
         <v>14</v>
       </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+      <c r="E21" t="s">
+        <v>104</v>
+      </c>
+      <c r="F21" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -1196,6 +1252,18 @@
       <c r="B22" t="s">
         <v>7</v>
       </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22">
+        <v>6</v>
+      </c>
+      <c r="E22">
+        <v>20250730</v>
+      </c>
+      <c r="F22">
+        <v>20250730</v>
+      </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -1233,8 +1301,8 @@
       <c r="E24">
         <v>20250718</v>
       </c>
-      <c r="F24" t="s">
-        <v>104</v>
+      <c r="F24">
+        <v>20250806</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
@@ -1463,6 +1531,12 @@
       <c r="B34" t="s">
         <v>7</v>
       </c>
+      <c r="C34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
       <c r="E34">
         <v>20250709</v>
       </c>
@@ -1486,6 +1560,9 @@
       <c r="E35">
         <v>20250709</v>
       </c>
+      <c r="F35">
+        <v>20250725</v>
+      </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
@@ -1610,6 +1687,9 @@
       <c r="E40">
         <v>20250707</v>
       </c>
+      <c r="F40">
+        <v>20250725</v>
+      </c>
       <c r="G40">
         <v>20250718</v>
       </c>
@@ -1665,6 +1745,9 @@
       <c r="E42">
         <v>20250711</v>
       </c>
+      <c r="F42">
+        <v>20250725</v>
+      </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
@@ -1742,6 +1825,18 @@
       <c r="B46" t="s">
         <v>7</v>
       </c>
+      <c r="C46" t="s">
+        <v>36</v>
+      </c>
+      <c r="D46">
+        <v>6</v>
+      </c>
+      <c r="E46">
+        <v>20250725</v>
+      </c>
+      <c r="F46">
+        <v>20250728</v>
+      </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
@@ -1830,6 +1925,18 @@
       <c r="B51" t="s">
         <v>9</v>
       </c>
+      <c r="C51" t="s">
+        <v>61</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51" t="s">
+        <v>104</v>
+      </c>
+      <c r="F51" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
@@ -2061,8 +2168,8 @@
       <c r="E61">
         <v>20250704</v>
       </c>
-      <c r="F61" t="s">
-        <v>104</v>
+      <c r="F61">
+        <v>20250806</v>
       </c>
       <c r="G61">
         <v>20250716</v>
@@ -2317,6 +2424,9 @@
       <c r="E72">
         <v>20250714</v>
       </c>
+      <c r="F72">
+        <v>20250725</v>
+      </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
@@ -2340,6 +2450,2925 @@
       <c r="G73">
         <v>20250718</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC495107-5DCB-4D40-8ECF-8F99937158A8}">
+  <dimension ref="A1:M73"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M73"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" customWidth="1"/>
+    <col min="9" max="10" width="17" customWidth="1"/>
+    <col min="11" max="11" width="14.83203125" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6">
+        <v>20250716</v>
+      </c>
+      <c r="F2">
+        <v>20250718</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6">
+        <v>20250716</v>
+      </c>
+      <c r="F3">
+        <v>20250716</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6">
+        <v>20250714</v>
+      </c>
+      <c r="F4">
+        <v>20250718</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6">
+        <v>20250709</v>
+      </c>
+      <c r="F5">
+        <v>20250714</v>
+      </c>
+      <c r="G5" t="s">
+        <v>105</v>
+      </c>
+      <c r="H5" t="s">
+        <v>105</v>
+      </c>
+      <c r="I5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="6">
+        <v>2</v>
+      </c>
+      <c r="E6" s="6">
+        <v>20250718</v>
+      </c>
+      <c r="F6">
+        <v>20250725</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="6">
+        <v>2</v>
+      </c>
+      <c r="E7" s="6">
+        <v>20250714</v>
+      </c>
+      <c r="F7">
+        <v>20250716</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="6">
+        <v>2</v>
+      </c>
+      <c r="E8" s="6">
+        <v>20250716</v>
+      </c>
+      <c r="F8">
+        <v>20250721</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="6">
+        <v>2</v>
+      </c>
+      <c r="E9" s="6">
+        <v>20250711</v>
+      </c>
+      <c r="F9">
+        <v>20250711</v>
+      </c>
+      <c r="G9" t="s">
+        <v>107</v>
+      </c>
+      <c r="H9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>20250709</v>
+      </c>
+      <c r="F10">
+        <v>20250721</v>
+      </c>
+      <c r="G10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>20250709</v>
+      </c>
+      <c r="F11">
+        <v>20250709</v>
+      </c>
+      <c r="G11" t="s">
+        <v>106</v>
+      </c>
+      <c r="H11" t="s">
+        <v>105</v>
+      </c>
+      <c r="I11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>20250711</v>
+      </c>
+      <c r="F12">
+        <v>20250716</v>
+      </c>
+      <c r="G12" t="s">
+        <v>107</v>
+      </c>
+      <c r="H12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>20250709</v>
+      </c>
+      <c r="F13">
+        <v>20250709</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="6">
+        <v>4</v>
+      </c>
+      <c r="E14" s="6">
+        <v>20250714</v>
+      </c>
+      <c r="F14">
+        <v>20250716</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="6">
+        <v>4</v>
+      </c>
+      <c r="E15" s="6">
+        <v>20250709</v>
+      </c>
+      <c r="F15">
+        <v>20250709</v>
+      </c>
+      <c r="G15" t="s">
+        <v>105</v>
+      </c>
+      <c r="H15" t="s">
+        <v>105</v>
+      </c>
+      <c r="I15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="6">
+        <v>4</v>
+      </c>
+      <c r="E16" s="6">
+        <v>20250716</v>
+      </c>
+      <c r="F16">
+        <v>20250716</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="6">
+        <v>4</v>
+      </c>
+      <c r="E17" s="6">
+        <v>20250709</v>
+      </c>
+      <c r="F17">
+        <v>20250716</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="4">
+        <v>5</v>
+      </c>
+      <c r="E18" s="4">
+        <v>20250714</v>
+      </c>
+      <c r="F18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="4">
+        <v>5</v>
+      </c>
+      <c r="E19" s="4">
+        <v>20250718</v>
+      </c>
+      <c r="F19">
+        <v>20250718</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="4">
+        <v>5</v>
+      </c>
+      <c r="E20" s="4">
+        <v>20250714</v>
+      </c>
+      <c r="F20">
+        <v>20250716</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="4">
+        <v>5</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="4">
+        <v>6</v>
+      </c>
+      <c r="E22" s="4">
+        <v>20250730</v>
+      </c>
+      <c r="F22">
+        <v>20250730</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="4">
+        <v>6</v>
+      </c>
+      <c r="E23" s="4">
+        <v>20250714</v>
+      </c>
+      <c r="F23">
+        <v>20250716</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="4">
+        <v>6</v>
+      </c>
+      <c r="E24" s="4">
+        <v>20250718</v>
+      </c>
+      <c r="F24">
+        <v>20250806</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="4">
+        <v>6</v>
+      </c>
+      <c r="E25" s="4">
+        <v>20250714</v>
+      </c>
+      <c r="F25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="7">
+        <v>1</v>
+      </c>
+      <c r="E26" s="7">
+        <v>20250711</v>
+      </c>
+      <c r="F26">
+        <v>20250711</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="7">
+        <v>1</v>
+      </c>
+      <c r="E27" s="7">
+        <v>20250711</v>
+      </c>
+      <c r="F27">
+        <v>20250711</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="7">
+        <v>1</v>
+      </c>
+      <c r="E28" s="7">
+        <v>20250718</v>
+      </c>
+      <c r="F28" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="7">
+        <v>1</v>
+      </c>
+      <c r="E29" s="7">
+        <v>20250718</v>
+      </c>
+      <c r="F29">
+        <v>20250718</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>20250707</v>
+      </c>
+      <c r="F30">
+        <v>20250714</v>
+      </c>
+      <c r="G30" s="4">
+        <v>20250916</v>
+      </c>
+      <c r="H30" s="4">
+        <v>20250916</v>
+      </c>
+      <c r="I30" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31">
+        <v>20250630</v>
+      </c>
+      <c r="F31">
+        <v>20250704</v>
+      </c>
+      <c r="G31">
+        <v>20250915</v>
+      </c>
+      <c r="H31">
+        <v>20250915</v>
+      </c>
+      <c r="I31" s="4">
+        <v>20250916</v>
+      </c>
+      <c r="L31" s="4"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32">
+        <v>20250704</v>
+      </c>
+      <c r="F32">
+        <v>20250704</v>
+      </c>
+      <c r="G32">
+        <v>20250915</v>
+      </c>
+      <c r="H32">
+        <v>20250915</v>
+      </c>
+      <c r="I32" s="4">
+        <v>20250916</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33">
+        <v>20250630</v>
+      </c>
+      <c r="F33">
+        <v>20250702</v>
+      </c>
+      <c r="G33">
+        <v>20250915</v>
+      </c>
+      <c r="H33">
+        <v>20250915</v>
+      </c>
+      <c r="I33" s="4">
+        <v>20250916</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" s="7">
+        <v>3</v>
+      </c>
+      <c r="E34" s="7">
+        <v>20250709</v>
+      </c>
+      <c r="F34">
+        <v>20250718</v>
+      </c>
+      <c r="G34" t="s">
+        <v>105</v>
+      </c>
+      <c r="H34" t="s">
+        <v>105</v>
+      </c>
+      <c r="I34" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D35" s="7">
+        <v>3</v>
+      </c>
+      <c r="E35" s="7">
+        <v>20250709</v>
+      </c>
+      <c r="F35">
+        <v>20250725</v>
+      </c>
+      <c r="G35" t="s">
+        <v>107</v>
+      </c>
+      <c r="H35" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D36" s="7">
+        <v>3</v>
+      </c>
+      <c r="E36" s="7">
+        <v>20250709</v>
+      </c>
+      <c r="F36">
+        <v>20250709</v>
+      </c>
+      <c r="G36" t="s">
+        <v>107</v>
+      </c>
+      <c r="H36" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D37" s="7">
+        <v>3</v>
+      </c>
+      <c r="E37" s="7">
+        <v>20250704</v>
+      </c>
+      <c r="F37">
+        <v>20250707</v>
+      </c>
+      <c r="G37">
+        <v>20250915</v>
+      </c>
+      <c r="H37">
+        <v>20250915</v>
+      </c>
+      <c r="I37" s="4">
+        <v>20250916</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38">
+        <v>4</v>
+      </c>
+      <c r="E38">
+        <v>20250707</v>
+      </c>
+      <c r="F38">
+        <v>20250716</v>
+      </c>
+      <c r="G38" s="5">
+        <v>20250916</v>
+      </c>
+      <c r="H38" s="5">
+        <v>20250916</v>
+      </c>
+      <c r="I38" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" t="s">
+        <v>36</v>
+      </c>
+      <c r="D39">
+        <v>4</v>
+      </c>
+      <c r="E39">
+        <v>20250702</v>
+      </c>
+      <c r="F39">
+        <v>20250702</v>
+      </c>
+      <c r="G39">
+        <v>20250915</v>
+      </c>
+      <c r="H39">
+        <v>20250915</v>
+      </c>
+      <c r="I39" s="4">
+        <v>20250916</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" t="s">
+        <v>36</v>
+      </c>
+      <c r="D40">
+        <v>4</v>
+      </c>
+      <c r="E40">
+        <v>20250707</v>
+      </c>
+      <c r="F40">
+        <v>20250725</v>
+      </c>
+      <c r="G40" s="5">
+        <v>20250916</v>
+      </c>
+      <c r="H40" s="5">
+        <v>20250916</v>
+      </c>
+      <c r="I40" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" t="s">
+        <v>36</v>
+      </c>
+      <c r="D41">
+        <v>4</v>
+      </c>
+      <c r="E41">
+        <v>20250702</v>
+      </c>
+      <c r="F41">
+        <v>20250702</v>
+      </c>
+      <c r="G41" s="4">
+        <v>20250915</v>
+      </c>
+      <c r="H41" s="4">
+        <v>20250915</v>
+      </c>
+      <c r="I41" s="4">
+        <v>20250916</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D42" s="7">
+        <v>5</v>
+      </c>
+      <c r="E42" s="7">
+        <v>20250711</v>
+      </c>
+      <c r="F42">
+        <v>20250725</v>
+      </c>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D43" s="7">
+        <v>5</v>
+      </c>
+      <c r="E43" s="7">
+        <v>20250709</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="I43" s="4"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D44" s="7">
+        <v>5</v>
+      </c>
+      <c r="E44" s="7">
+        <v>20250716</v>
+      </c>
+      <c r="F44">
+        <v>20250716</v>
+      </c>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D45" s="7">
+        <v>5</v>
+      </c>
+      <c r="E45" s="7">
+        <v>20250704</v>
+      </c>
+      <c r="F45">
+        <v>20250707</v>
+      </c>
+      <c r="G45" s="4">
+        <v>20250915</v>
+      </c>
+      <c r="H45" s="4">
+        <v>20250915</v>
+      </c>
+      <c r="I45" s="4">
+        <v>20250916</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>56</v>
+      </c>
+      <c r="B46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" t="s">
+        <v>36</v>
+      </c>
+      <c r="D46">
+        <v>6</v>
+      </c>
+      <c r="E46">
+        <v>20250725</v>
+      </c>
+      <c r="F46">
+        <v>20250728</v>
+      </c>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>57</v>
+      </c>
+      <c r="B47" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" t="s">
+        <v>36</v>
+      </c>
+      <c r="D47">
+        <v>6</v>
+      </c>
+      <c r="E47">
+        <v>20250716</v>
+      </c>
+      <c r="F47">
+        <v>20250718</v>
+      </c>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>58</v>
+      </c>
+      <c r="B48" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" t="s">
+        <v>36</v>
+      </c>
+      <c r="D48">
+        <v>6</v>
+      </c>
+      <c r="E48">
+        <v>20250718</v>
+      </c>
+      <c r="F48">
+        <v>20250721</v>
+      </c>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>59</v>
+      </c>
+      <c r="B49" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" t="s">
+        <v>36</v>
+      </c>
+      <c r="D49">
+        <v>6</v>
+      </c>
+      <c r="E49">
+        <v>20250711</v>
+      </c>
+      <c r="F49">
+        <v>20250714</v>
+      </c>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>60</v>
+      </c>
+      <c r="B50" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" t="s">
+        <v>61</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>20250711</v>
+      </c>
+      <c r="F50">
+        <v>20250711</v>
+      </c>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>62</v>
+      </c>
+      <c r="B51" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" t="s">
+        <v>61</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51" t="s">
+        <v>104</v>
+      </c>
+      <c r="F51" t="s">
+        <v>104</v>
+      </c>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>63</v>
+      </c>
+      <c r="B52" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" t="s">
+        <v>61</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>20250714</v>
+      </c>
+      <c r="F52">
+        <v>20250716</v>
+      </c>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>64</v>
+      </c>
+      <c r="B53" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" t="s">
+        <v>61</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>20250707</v>
+      </c>
+      <c r="F53">
+        <v>20250714</v>
+      </c>
+      <c r="G53" s="5">
+        <v>20250916</v>
+      </c>
+      <c r="H53" s="5">
+        <v>20250916</v>
+      </c>
+      <c r="I53" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>65</v>
+      </c>
+      <c r="B54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" t="s">
+        <v>61</v>
+      </c>
+      <c r="D54">
+        <v>2</v>
+      </c>
+      <c r="E54">
+        <v>20250709</v>
+      </c>
+      <c r="F54">
+        <v>20250709</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="I54" s="4"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" t="s">
+        <v>61</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+      <c r="E55">
+        <v>20250707</v>
+      </c>
+      <c r="F55">
+        <v>20250714</v>
+      </c>
+      <c r="G55" s="5">
+        <v>20250916</v>
+      </c>
+      <c r="H55" s="5">
+        <v>20250916</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>67</v>
+      </c>
+      <c r="B56" t="s">
+        <v>11</v>
+      </c>
+      <c r="C56" t="s">
+        <v>61</v>
+      </c>
+      <c r="D56">
+        <v>2</v>
+      </c>
+      <c r="E56">
+        <v>20250714</v>
+      </c>
+      <c r="F56">
+        <v>20250721</v>
+      </c>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>68</v>
+      </c>
+      <c r="B57" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57" t="s">
+        <v>61</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57">
+        <v>20250704</v>
+      </c>
+      <c r="F57">
+        <v>20250704</v>
+      </c>
+      <c r="G57" s="4">
+        <v>20250915</v>
+      </c>
+      <c r="H57" s="4">
+        <v>20250915</v>
+      </c>
+      <c r="I57" s="4">
+        <v>20250916</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D58" s="8">
+        <v>3</v>
+      </c>
+      <c r="E58" s="8">
+        <v>20250709</v>
+      </c>
+      <c r="F58">
+        <v>20250709</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="I58" s="4"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D59" s="8">
+        <v>3</v>
+      </c>
+      <c r="E59" s="8">
+        <v>20250707</v>
+      </c>
+      <c r="F59">
+        <v>20250716</v>
+      </c>
+      <c r="G59" s="5">
+        <v>20250916</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="I59" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D60" s="8">
+        <v>3</v>
+      </c>
+      <c r="E60" s="8">
+        <v>20250718</v>
+      </c>
+      <c r="F60">
+        <v>20250718</v>
+      </c>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D61" s="8">
+        <v>3</v>
+      </c>
+      <c r="E61" s="8">
+        <v>20250704</v>
+      </c>
+      <c r="F61">
+        <v>20250806</v>
+      </c>
+      <c r="G61" s="4">
+        <v>20250915</v>
+      </c>
+      <c r="H61" s="4">
+        <v>20250915</v>
+      </c>
+      <c r="I61" s="4">
+        <v>20250916</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D62" s="8">
+        <v>4</v>
+      </c>
+      <c r="E62" s="8">
+        <v>20250711</v>
+      </c>
+      <c r="F62">
+        <v>20250721</v>
+      </c>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D63" s="8">
+        <v>4</v>
+      </c>
+      <c r="E63" s="8">
+        <v>20250704</v>
+      </c>
+      <c r="F63">
+        <v>20250704</v>
+      </c>
+      <c r="G63" s="4">
+        <v>20250915</v>
+      </c>
+      <c r="H63" s="4">
+        <v>20250915</v>
+      </c>
+      <c r="I63" s="4">
+        <v>20250916</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D64" s="8">
+        <v>4</v>
+      </c>
+      <c r="E64" s="8">
+        <v>20250709</v>
+      </c>
+      <c r="F64">
+        <v>20250714</v>
+      </c>
+      <c r="G64" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H64" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="I64" s="4"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D65" s="8">
+        <v>4</v>
+      </c>
+      <c r="E65" s="8">
+        <v>20250704</v>
+      </c>
+      <c r="F65">
+        <v>20250718</v>
+      </c>
+      <c r="G65" s="4">
+        <v>20250915</v>
+      </c>
+      <c r="H65" s="4">
+        <v>20250915</v>
+      </c>
+      <c r="I65" s="4">
+        <v>20250916</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D66" s="8">
+        <v>4</v>
+      </c>
+      <c r="E66" s="8">
+        <v>20250716</v>
+      </c>
+      <c r="F66">
+        <v>20250721</v>
+      </c>
+      <c r="G66" s="4"/>
+      <c r="H66" s="4"/>
+      <c r="I66" s="4"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D67" s="8">
+        <v>4</v>
+      </c>
+      <c r="E67" s="8">
+        <v>20250716</v>
+      </c>
+      <c r="F67">
+        <v>20250716</v>
+      </c>
+      <c r="G67" s="4"/>
+      <c r="H67" s="4"/>
+      <c r="I67" s="4"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D68" s="8">
+        <v>4</v>
+      </c>
+      <c r="E68" s="8">
+        <v>20250716</v>
+      </c>
+      <c r="F68">
+        <v>20250721</v>
+      </c>
+      <c r="G68" s="4"/>
+      <c r="H68" s="4"/>
+      <c r="I68" s="4"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A69" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D69" s="8">
+        <v>5</v>
+      </c>
+      <c r="E69" s="8">
+        <v>20250714</v>
+      </c>
+      <c r="F69">
+        <v>20250716</v>
+      </c>
+      <c r="G69" s="4"/>
+      <c r="H69" s="4"/>
+      <c r="I69" s="4"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>81</v>
+      </c>
+      <c r="B70" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" t="s">
+        <v>61</v>
+      </c>
+      <c r="D70">
+        <v>6</v>
+      </c>
+      <c r="E70">
+        <v>20250711</v>
+      </c>
+      <c r="F70">
+        <v>20250711</v>
+      </c>
+      <c r="G70" s="4"/>
+      <c r="H70" s="4"/>
+      <c r="I70" s="4"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>82</v>
+      </c>
+      <c r="B71" t="s">
+        <v>9</v>
+      </c>
+      <c r="C71" t="s">
+        <v>61</v>
+      </c>
+      <c r="D71">
+        <v>6</v>
+      </c>
+      <c r="E71">
+        <v>20250711</v>
+      </c>
+      <c r="F71">
+        <v>20250714</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>83</v>
+      </c>
+      <c r="B72" t="s">
+        <v>11</v>
+      </c>
+      <c r="C72" t="s">
+        <v>61</v>
+      </c>
+      <c r="D72">
+        <v>6</v>
+      </c>
+      <c r="E72">
+        <v>20250714</v>
+      </c>
+      <c r="F72">
+        <v>20250725</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>84</v>
+      </c>
+      <c r="B73" t="s">
+        <v>14</v>
+      </c>
+      <c r="C73" t="s">
+        <v>61</v>
+      </c>
+      <c r="D73">
+        <v>6</v>
+      </c>
+      <c r="E73">
+        <v>20250707</v>
+      </c>
+      <c r="F73">
+        <v>20250707</v>
+      </c>
+      <c r="G73" t="s">
+        <v>105</v>
+      </c>
+      <c r="H73" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DE8EF74-6DE4-164A-A47F-EE2826182DA1}">
+  <dimension ref="A1:M70"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="15.83203125" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6">
+        <v>20250716</v>
+      </c>
+      <c r="F2">
+        <v>20250718</v>
+      </c>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6">
+        <v>20250716</v>
+      </c>
+      <c r="F3">
+        <v>20250716</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6">
+        <v>20250714</v>
+      </c>
+      <c r="F4">
+        <v>20250718</v>
+      </c>
+      <c r="G4" s="9">
+        <v>20250918</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6">
+        <v>20250709</v>
+      </c>
+      <c r="F5">
+        <v>20250714</v>
+      </c>
+      <c r="G5" s="9">
+        <v>20250918</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="6">
+        <v>2</v>
+      </c>
+      <c r="E6" s="6">
+        <v>20250718</v>
+      </c>
+      <c r="F6">
+        <v>20250725</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="6">
+        <v>2</v>
+      </c>
+      <c r="E7" s="6">
+        <v>20250714</v>
+      </c>
+      <c r="F7">
+        <v>20250716</v>
+      </c>
+      <c r="G7" s="9">
+        <v>20250918</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="6">
+        <v>2</v>
+      </c>
+      <c r="E8" s="6">
+        <v>20250716</v>
+      </c>
+      <c r="F8">
+        <v>20250721</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="6">
+        <v>2</v>
+      </c>
+      <c r="E9" s="6">
+        <v>20250711</v>
+      </c>
+      <c r="F9">
+        <v>20250711</v>
+      </c>
+      <c r="G9" s="9">
+        <v>20250918</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="6">
+        <v>4</v>
+      </c>
+      <c r="E10" s="6">
+        <v>20250714</v>
+      </c>
+      <c r="F10">
+        <v>20250716</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="6">
+        <v>4</v>
+      </c>
+      <c r="E11" s="6">
+        <v>20250709</v>
+      </c>
+      <c r="F11">
+        <v>20250709</v>
+      </c>
+      <c r="G11" s="9">
+        <v>20250918</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="6">
+        <v>4</v>
+      </c>
+      <c r="E12" s="6">
+        <v>20250716</v>
+      </c>
+      <c r="F12">
+        <v>20250716</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="6">
+        <v>4</v>
+      </c>
+      <c r="E13" s="6">
+        <v>20250709</v>
+      </c>
+      <c r="F13">
+        <v>20250716</v>
+      </c>
+      <c r="G13" s="9">
+        <v>20250918</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="7">
+        <v>1</v>
+      </c>
+      <c r="E14" s="7">
+        <v>20250711</v>
+      </c>
+      <c r="F14">
+        <v>20250711</v>
+      </c>
+      <c r="G14" s="9">
+        <v>20250918</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="7">
+        <v>1</v>
+      </c>
+      <c r="E15" s="7">
+        <v>20250711</v>
+      </c>
+      <c r="F15">
+        <v>20250711</v>
+      </c>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="7">
+        <v>1</v>
+      </c>
+      <c r="E16" s="7">
+        <v>20250718</v>
+      </c>
+      <c r="F16" t="s">
+        <v>104</v>
+      </c>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="7">
+        <v>1</v>
+      </c>
+      <c r="E17" s="7">
+        <v>20250718</v>
+      </c>
+      <c r="F17">
+        <v>20250718</v>
+      </c>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="7">
+        <v>3</v>
+      </c>
+      <c r="E18" s="7">
+        <v>20250709</v>
+      </c>
+      <c r="F18">
+        <v>20250718</v>
+      </c>
+      <c r="G18" s="9">
+        <v>20250918</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="7">
+        <v>3</v>
+      </c>
+      <c r="E19" s="7">
+        <v>20250709</v>
+      </c>
+      <c r="F19">
+        <v>20250725</v>
+      </c>
+      <c r="G19" s="9">
+        <v>20250918</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="7">
+        <v>3</v>
+      </c>
+      <c r="E20" s="7">
+        <v>20250709</v>
+      </c>
+      <c r="F20">
+        <v>20250709</v>
+      </c>
+      <c r="G20" s="9">
+        <v>20250918</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="7">
+        <v>3</v>
+      </c>
+      <c r="E21" s="7">
+        <v>20250704</v>
+      </c>
+      <c r="F21">
+        <v>20250707</v>
+      </c>
+      <c r="G21" s="9">
+        <v>20250918</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="7">
+        <v>5</v>
+      </c>
+      <c r="E22" s="7">
+        <v>20250711</v>
+      </c>
+      <c r="F22">
+        <v>20250725</v>
+      </c>
+      <c r="G22" s="9">
+        <v>20250918</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="7">
+        <v>5</v>
+      </c>
+      <c r="E23" s="7">
+        <v>20250709</v>
+      </c>
+      <c r="G23" s="9">
+        <v>20250918</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="7">
+        <v>5</v>
+      </c>
+      <c r="E24" s="7">
+        <v>20250716</v>
+      </c>
+      <c r="F24">
+        <v>20250716</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="7">
+        <v>5</v>
+      </c>
+      <c r="E25" s="7">
+        <v>20250704</v>
+      </c>
+      <c r="F25">
+        <v>20250707</v>
+      </c>
+      <c r="G25" s="9">
+        <v>20250918</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="8">
+        <v>3</v>
+      </c>
+      <c r="E26" s="8">
+        <v>20250709</v>
+      </c>
+      <c r="F26">
+        <v>20250709</v>
+      </c>
+      <c r="G26" s="9">
+        <v>20250918</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="8">
+        <v>3</v>
+      </c>
+      <c r="E27" s="8">
+        <v>20250707</v>
+      </c>
+      <c r="F27">
+        <v>20250716</v>
+      </c>
+      <c r="G27" s="9">
+        <v>20250918</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" s="8">
+        <v>3</v>
+      </c>
+      <c r="E28" s="8">
+        <v>20250718</v>
+      </c>
+      <c r="F28">
+        <v>20250718</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="8">
+        <v>3</v>
+      </c>
+      <c r="E29" s="8">
+        <v>20250704</v>
+      </c>
+      <c r="F29">
+        <v>20250806</v>
+      </c>
+      <c r="G29" s="9">
+        <v>20250918</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="8">
+        <v>4</v>
+      </c>
+      <c r="E30" s="8">
+        <v>20250711</v>
+      </c>
+      <c r="F30">
+        <v>20250721</v>
+      </c>
+      <c r="G30" s="9">
+        <v>20250918</v>
+      </c>
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" s="8">
+        <v>4</v>
+      </c>
+      <c r="E31" s="8">
+        <v>20250704</v>
+      </c>
+      <c r="F31">
+        <v>20250704</v>
+      </c>
+      <c r="G31" s="9">
+        <v>20250918</v>
+      </c>
+      <c r="I31" s="4"/>
+      <c r="L31" s="4"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="8">
+        <v>4</v>
+      </c>
+      <c r="E32" s="8">
+        <v>20250709</v>
+      </c>
+      <c r="F32">
+        <v>20250714</v>
+      </c>
+      <c r="G32" s="9">
+        <v>20250918</v>
+      </c>
+      <c r="I32" s="4"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="8">
+        <v>4</v>
+      </c>
+      <c r="E33" s="8">
+        <v>20250704</v>
+      </c>
+      <c r="F33">
+        <v>20250718</v>
+      </c>
+      <c r="G33" s="9">
+        <v>20250918</v>
+      </c>
+      <c r="I33" s="4"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" s="8">
+        <v>4</v>
+      </c>
+      <c r="E34" s="8">
+        <v>20250716</v>
+      </c>
+      <c r="F34">
+        <v>20250721</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35" s="8">
+        <v>4</v>
+      </c>
+      <c r="E35" s="8">
+        <v>20250716</v>
+      </c>
+      <c r="F35">
+        <v>20250716</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D36" s="8">
+        <v>4</v>
+      </c>
+      <c r="E36" s="8">
+        <v>20250716</v>
+      </c>
+      <c r="F36">
+        <v>20250721</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D37" s="8">
+        <v>5</v>
+      </c>
+      <c r="E37" s="8">
+        <v>20250714</v>
+      </c>
+      <c r="F37">
+        <v>20250716</v>
+      </c>
+      <c r="G37" s="9">
+        <v>20250918</v>
+      </c>
+      <c r="I37" s="4"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I39" s="4"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="4"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G55" s="5"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="4"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="4"/>
+      <c r="I63" s="4"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+      <c r="G65" s="4"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="4"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="4"/>
+      <c r="H66" s="4"/>
+      <c r="I66" s="4"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="4"/>
+      <c r="G67" s="4"/>
+      <c r="H67" s="4"/>
+      <c r="I67" s="4"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="4"/>
+      <c r="G68" s="4"/>
+      <c r="H68" s="4"/>
+      <c r="I68" s="4"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A69" s="4"/>
+      <c r="B69" s="4"/>
+      <c r="C69" s="4"/>
+      <c r="D69" s="4"/>
+      <c r="E69" s="4"/>
+      <c r="F69" s="4"/>
+      <c r="G69" s="4"/>
+      <c r="H69" s="4"/>
+      <c r="I69" s="4"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G70" s="4"/>
+      <c r="H70" s="4"/>
+      <c r="I70" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>